<commit_message>
Just loads of stuff I've forgotten to commit
</commit_message>
<xml_diff>
--- a/time_shift/original_data/replicate_decision.xlsx
+++ b/time_shift/original_data/replicate_decision.xlsx
@@ -90,7 +90,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -98,316 +98,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -697,7 +387,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -778,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -826,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1157,10 +847,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E25">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>